<commit_message>
Kan geen records uit de databank halen , login werkt wel
</commit_message>
<xml_diff>
--- a/scrumVideotheek.xlsx
+++ b/scrumVideotheek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gooss\Desktop\CubeBurster\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school 6ib\C#\cubeburster\CubeBurster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1A9D93-243F-4638-81BD-9133098D35F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A58849-F236-429C-925B-EB7674CE0F46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="64">
   <si>
     <t>Als ontlener wil ik een lijst van alle films kunnen zien zodat ik weet welke films ik kan kiezen</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>Kieron/Rein</t>
+  </si>
+  <si>
+    <t>sepp/Kieron</t>
+  </si>
+  <si>
+    <t>2u30m</t>
+  </si>
+  <si>
+    <t>Kunnen geen induviduele gegevens uit records halen</t>
   </si>
 </sst>
 </file>
@@ -1199,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1211,9 +1220,10 @@
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
@@ -1227,7 +1237,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1241,7 +1251,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1255,15 +1265,24 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1271,7 +1290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1279,7 +1298,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1287,7 +1306,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1295,7 +1314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1303,7 +1322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1330,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1346,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1335,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1343,7 +1362,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1351,7 +1370,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>